<commit_message>
hasta histograma de variable gastos
</commit_message>
<xml_diff>
--- a/Métodos Estadísticos  posgrado/TABLAPESOS.xlsx
+++ b/Métodos Estadísticos  posgrado/TABLAPESOS.xlsx
@@ -1,40 +1,196 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\METODOSESTADISTICOS\CLASE1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\GitHub\Metodos-estadisticos\Métodos Estadísticos  posgrado\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED2A195-FC05-42AE-86EF-52720E15BB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11985"/>
+    <workbookView xWindow="345" yWindow="2850" windowWidth="22050" windowHeight="12270" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={7D85765D-82AD-44F3-896F-BAEAF304D524}</author>
+  </authors>
+  <commentList>
+    <comment ref="G44" authorId="0" shapeId="0" xr:uid="{7D85765D-82AD-44F3-896F-BAEAF304D524}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    El 62% de las mujeres de la muestra pesan entre 53 y 64 kg</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>pesos</t>
+  </si>
+  <si>
+    <t>longitud de intervalo</t>
+  </si>
+  <si>
+    <t>minimo</t>
+  </si>
+  <si>
+    <t>maximo</t>
+  </si>
+  <si>
+    <t>valores maximos de los intervalos</t>
+  </si>
+  <si>
+    <t>Clase</t>
+  </si>
+  <si>
+    <t>y mayor...</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>% acumulada</t>
+  </si>
+  <si>
+    <t>intervalo</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>53-55</t>
+  </si>
+  <si>
+    <t>56-58</t>
+  </si>
+  <si>
+    <t>59-61</t>
+  </si>
+  <si>
+    <t>62-64</t>
+  </si>
+  <si>
+    <t>65-67</t>
+  </si>
+  <si>
+    <t>68-70</t>
+  </si>
+  <si>
+    <t>71-73</t>
+  </si>
+  <si>
+    <t>Fi</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>absoluta</t>
+  </si>
+  <si>
+    <t>abs. acumul.</t>
+  </si>
+  <si>
+    <t>relativa</t>
+  </si>
+  <si>
+    <t>rel. acumul.</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Error típico</t>
+  </si>
+  <si>
+    <t>Mediana</t>
+  </si>
+  <si>
+    <t>Moda</t>
+  </si>
+  <si>
+    <t>Desviación estándar</t>
+  </si>
+  <si>
+    <t>Varianza de la muestra</t>
+  </si>
+  <si>
+    <t>Curtosis</t>
+  </si>
+  <si>
+    <t>Coeficiente de asimetría</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Mínimo</t>
+  </si>
+  <si>
+    <t>Máximo</t>
+  </si>
+  <si>
+    <t>Suma</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -50,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -58,12 +214,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -79,6 +264,979 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>% de pesos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Hoja1!$C$28:$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>53-55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56-58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59-61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62-64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>65-67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68-70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71-73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$D$28:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4114-4767-B027-0B411925F75C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1894915424"/>
+        <c:axId val="1894918752"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1894915424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1894918752"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1894918752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1894915424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{853BDC03-4704-44D2-9B6C-A9BA2E4B92F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Andrés Felipe Beltrán Rodriguez" id="{2F4F7D82-2BAD-4418-BB35-2FA6C27B9C6C}" userId="Andrés Felipe Beltrán Rodriguez" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +1500,864 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G44" dT="2021-10-26T11:51:02.05" personId="{2F4F7D82-2BAD-4418-BB35-2FA6C27B9C6C}" id="{7D85765D-82AD-44F3-896F-BAEAF304D524}">
+    <text>El 62% de las mujeres de la muestra pesan entre 53 y 64 kg</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0572E4D6-F05F-4EF2-BD16-32CC0A731305}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A8">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4BB1B74-FFF3-4ED3-86C4-CC1B6F6C8E1A}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="5"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.58484255687024922</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="2">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.1354613788943233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2">
+        <v>17.102040816326536</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-7.1372264741106584E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2">
+        <v>-0.20235078164503226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="3">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A51" sqref="A1:A51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>65</v>
+      </c>
+      <c r="C2">
+        <f>MIN(A2:A51)</f>
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>63</v>
+      </c>
+      <c r="C3">
+        <f>MAX(A2:A51)</f>
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>65</v>
+      </c>
+      <c r="C4">
+        <f>(C3-C2)/7</f>
+        <v>2.7142857142857144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2">
+        <v>63.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.58484255687024922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>55</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="2">
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>53</v>
+      </c>
+      <c r="C8">
+        <v>58</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>61</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="2">
+        <v>4.1354613788943233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="2">
+        <v>17.102040816326536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>61</v>
+      </c>
+      <c r="C11">
+        <v>67</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="2">
+        <v>-7.1372264741106584E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="C12">
+        <v>70</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="2">
+        <v>-0.20235078164503226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>65</v>
+      </c>
+      <c r="C13">
+        <v>73</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>64</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>72</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>68</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1">
+        <v>55</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17:E23" si="0">D17/50*100</f>
+        <v>4</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>55</v>
+      </c>
+      <c r="C18" s="1">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2">
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>60</v>
+      </c>
+      <c r="C20" s="1">
+        <v>64</v>
+      </c>
+      <c r="D20" s="2">
+        <v>15</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>62</v>
+      </c>
+      <c r="C21" s="1">
+        <v>67</v>
+      </c>
+      <c r="D21" s="2">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>64</v>
+      </c>
+      <c r="C22" s="1">
+        <v>70</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1">
+        <v>73</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>64</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>66</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>63</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>59</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>61</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <f>D41/50</f>
+        <v>0.04</v>
+      </c>
+      <c r="F41">
+        <f>SUM(D41)</f>
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <f>E41</f>
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42">
+        <v>5</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42:E47" si="1">D42/50</f>
+        <v>0.1</v>
+      </c>
+      <c r="F42">
+        <f>SUM(D41:D42)</f>
+        <v>7</v>
+      </c>
+      <c r="G42">
+        <f>E42+E41</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>64</v>
+      </c>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>9</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="F43">
+        <f>SUM(D41:D43)</f>
+        <v>16</v>
+      </c>
+      <c r="G43">
+        <f>E43+E42+E41</f>
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44">
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="F44">
+        <f>SUM(D41:D44)</f>
+        <v>31</v>
+      </c>
+      <c r="G44">
+        <f>E44+E43+E42+E41</f>
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>69</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>12</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0.24</v>
+      </c>
+      <c r="F45">
+        <f>SUM(D41:D45)</f>
+        <v>43</v>
+      </c>
+      <c r="G45">
+        <f>E45+E44+E43+E42+E41</f>
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>67</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F46">
+        <f>SUM(D41:D46)</f>
+        <v>48</v>
+      </c>
+      <c r="G46">
+        <f>E46+E45+E44+E43+E42+E41</f>
+        <v>0.95999999999999985</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="F47">
+        <f>SUM(D41:D47)</f>
+        <v>50</v>
+      </c>
+      <c r="G47">
+        <f>E47+E46+E45+E44+E43+E42+E41</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F42:F43 F44:F46" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64EB0A8B-F233-4B8B-BF5F-D12B965BB154}">
   <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A51"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>